<commit_message>
lots of updates to Part 2
</commit_message>
<xml_diff>
--- a/Part_2_tables/match_on_abstract_df_grouped.xlsx
+++ b/Part_2_tables/match_on_abstract_df_grouped.xlsx
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>71</v>
+        <v>7973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>